<commit_message>
new rds files and new metrics in excel files
</commit_message>
<xml_diff>
--- a/CM_results_Angie_7_datasets.xlsx
+++ b/CM_results_Angie_7_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/az/Documents/GitHub/Spring_2019_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F998FD5-7BE8-744B-805F-F0F3EC3479E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC29EE31-68EF-824A-BBDE-5E74088A9490}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="480" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rao_gm12878_5kb" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="50">
   <si>
     <t>Table 1</t>
   </si>
@@ -129,6 +129,54 @@
   </si>
   <si>
     <t>cannot scale data.Variable 'constant</t>
+  </si>
+  <si>
+    <t>total 111 predictors</t>
+  </si>
+  <si>
+    <t>2:112 by 2</t>
+  </si>
+  <si>
+    <t>final value used 74</t>
+  </si>
+  <si>
+    <t>accuracy at 74 is 0.6783</t>
+  </si>
+  <si>
+    <t>total 385 predictors</t>
+  </si>
+  <si>
+    <t>9:378 by 9</t>
+  </si>
+  <si>
+    <t>final value used 252</t>
+  </si>
+  <si>
+    <t>accuracy at 252 is 0.697127</t>
+  </si>
+  <si>
+    <t>5416 obs of 369 var</t>
+  </si>
+  <si>
+    <t>1354 obs of 369 var</t>
+  </si>
+  <si>
+    <t>total 368 predictors</t>
+  </si>
+  <si>
+    <t>9:369 by 9</t>
+  </si>
+  <si>
+    <t>final value used 297</t>
+  </si>
+  <si>
+    <t>accuracy at 74 is 0.71288</t>
+  </si>
+  <si>
+    <t>positive class</t>
+  </si>
+  <si>
+    <t>random</t>
   </si>
 </sst>
 </file>
@@ -2249,8 +2297,8 @@
   </sheetPr>
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2529,8 +2577,12 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="10"/>
@@ -2585,7 +2637,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2626,7 +2678,9 @@
         <v>3</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5">
+        <v>0.71479999999999999</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
@@ -2637,7 +2691,9 @@
         <v>4</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="C4" s="9">
+        <v>0.67390000000000005</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
@@ -2648,7 +2704,9 @@
         <v>5</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9">
+        <v>0.75570000000000004</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
@@ -2659,7 +2717,9 @@
         <v>6</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="C6" s="9">
+        <v>0.7026</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
@@ -2670,7 +2730,9 @@
         <v>7</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9">
+        <v>0.73399999999999999</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
@@ -2681,7 +2743,9 @@
         <v>8</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9">
+        <v>0.67390000000000005</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
@@ -2730,7 +2794,9 @@
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
@@ -2739,7 +2805,9 @@
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" s="11"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
@@ -2748,7 +2816,9 @@
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
@@ -2757,16 +2827,20 @@
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" s="11"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
@@ -2882,7 +2956,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A12" sqref="A12:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2923,8 +2997,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="5">
+        <v>0.68020000000000003</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.67179999999999995</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -2934,8 +3012,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="9">
+        <v>0.62409999999999999</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.60170000000000001</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -2945,8 +3027,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="9">
+        <v>0.73629999999999995</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.7419</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -2956,8 +3042,12 @@
         <v>6</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="9">
+        <v>0.66120000000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.64710000000000001</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -2967,8 +3057,12 @@
         <v>7</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="C7" s="9">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.69979999999999998</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -2978,8 +3072,12 @@
         <v>8</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="C8" s="9">
+        <v>0.62409999999999999</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.60170000000000001</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -3018,7 +3116,9 @@
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
@@ -3027,7 +3127,9 @@
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="D13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
@@ -3036,7 +3138,9 @@
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="11"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
@@ -3045,16 +3149,20 @@
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
@@ -3178,8 +3286,8 @@
   </sheetPr>
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="B3:E11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3220,7 +3328,9 @@
         <v>3</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5">
+        <v>0.71199999999999997</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
@@ -3231,7 +3341,9 @@
         <v>4</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="C4" s="9">
+        <v>0.64549999999999996</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
@@ -3242,7 +3354,9 @@
         <v>5</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9">
+        <v>0.77839999999999998</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
@@ -3253,7 +3367,9 @@
         <v>6</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="C6" s="9">
+        <v>0.6915</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
@@ -3264,7 +3380,9 @@
         <v>7</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9">
+        <v>0.74450000000000005</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
@@ -3275,7 +3393,9 @@
         <v>8</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9">
+        <v>0.64549999999999996</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
@@ -3315,7 +3435,9 @@
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
@@ -3324,7 +3446,9 @@
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="D13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
@@ -3333,7 +3457,9 @@
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="D14" s="11"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
@@ -3342,16 +3468,20 @@
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
@@ -3367,8 +3497,12 @@
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="14"/>
@@ -3376,8 +3510,12 @@
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="10"/>

</xml_diff>

<commit_message>
outfut txt files and rds files. Excel updated
</commit_message>
<xml_diff>
--- a/CM_results_Angie_7_datasets.xlsx
+++ b/CM_results_Angie_7_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/az/Documents/GitHub/Spring_2019_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC29EE31-68EF-824A-BBDE-5E74088A9490}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3367A7C4-C987-754B-BDA8-1FA12E42BC51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28080" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rao_gm12878_5kb" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="69">
   <si>
     <t>Table 1</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Logistic Regression a=.05</t>
-  </si>
-  <si>
-    <t>Matthews correlation coefficient</t>
   </si>
   <si>
     <t>SVM radial 
@@ -110,27 +107,12 @@
     <t>10:400 by 10</t>
   </si>
   <si>
-    <t>final value used 300</t>
-  </si>
-  <si>
-    <t>accuracy at 198 is 0.88569</t>
-  </si>
-  <si>
     <t>2082 obs of 408 var</t>
   </si>
   <si>
     <t>520 obs of 408 var</t>
   </si>
   <si>
-    <t>? 0.9544</t>
-  </si>
-  <si>
-    <t>error: object 'model' not found</t>
-  </si>
-  <si>
-    <t>cannot scale data.Variable 'constant</t>
-  </si>
-  <si>
     <t>total 111 predictors</t>
   </si>
   <si>
@@ -177,13 +159,91 @@
   </si>
   <si>
     <t>random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing </t>
+  </si>
+  <si>
+    <t>6096 obs of 172 var</t>
+  </si>
+  <si>
+    <t>1524 obs of 172 var</t>
+  </si>
+  <si>
+    <t>7736 obs of 180 var</t>
+  </si>
+  <si>
+    <t>1934 obs of 180 var</t>
+  </si>
+  <si>
+    <t>total 179 predictors</t>
+  </si>
+  <si>
+    <t>4:180 by 4</t>
+  </si>
+  <si>
+    <t>final value used 290</t>
+  </si>
+  <si>
+    <t>accuracy at 290 is 0.8847</t>
+  </si>
+  <si>
+    <t>total 171 predictors</t>
+  </si>
+  <si>
+    <t>4:172 by 4</t>
+  </si>
+  <si>
+    <t>final value used 68</t>
+  </si>
+  <si>
+    <t>accuracy at 68 is 0.7590</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trials </t>
+  </si>
+  <si>
+    <t>1:99 by 2</t>
+  </si>
+  <si>
+    <t>final value used trials=5</t>
+  </si>
+  <si>
+    <t>accuracy at 5 is 0.7352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive class </t>
+  </si>
+  <si>
+    <t>final value used 176</t>
+  </si>
+  <si>
+    <t>accuracy at 176 is 0.7032</t>
+  </si>
+  <si>
+    <t>final value used trials=7</t>
+  </si>
+  <si>
+    <t>accuracy at 5 is 0.6685</t>
+  </si>
+  <si>
+    <t>final value used trials=9</t>
+  </si>
+  <si>
+    <t>accuracy at 5 is 0.68039</t>
+  </si>
+  <si>
+    <t>accuracy at 5 is 0.67019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -199,6 +259,24 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -353,7 +431,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -416,6 +494,45 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,6 +670,55 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698734</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>193090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069105</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>188544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02DD7D0C-25DF-CA48-9190-DED03219223A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432534" y="3469690"/>
+          <a:ext cx="370371" cy="249454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -577,6 +743,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E96198-3F07-5241-B5E0-466D09FF6267}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432534" y="3469690"/>
+          <a:ext cx="370371" cy="249454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698734</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>193090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069105</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>188544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5E2F1AF-2F76-9942-AE0E-4A127C1C69D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -661,6 +876,55 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698734</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>193090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069105</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>188544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191BDFFB-E68F-6B48-96A5-E7E9AC54D70A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432534" y="3469690"/>
+          <a:ext cx="370371" cy="249454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -715,6 +979,55 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698734</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>193090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069105</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>188544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8104F1DB-E219-FE42-AFEB-E38AB0EC7390}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432534" y="3469690"/>
+          <a:ext cx="370371" cy="249454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -739,6 +1052,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78330A89-A62A-0B4F-9459-33F9AAA1C39E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432534" y="3469690"/>
+          <a:ext cx="370371" cy="249454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698734</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>193090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069105</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>188544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E69163-5FF2-304A-8072-B4FE723EBE03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -847,6 +1209,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB7C5D5E-34D2-2248-923E-CA5ED1BAE17A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4432534" y="3469690"/>
+          <a:ext cx="370371" cy="249454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698734</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>193090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069105</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>188544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B982F3-D022-724B-97BC-D557C366F2EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1960,8 +2371,8 @@
   </sheetPr>
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1992,7 +2403,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -2111,15 +2522,11 @@
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="13"/>
       <c r="B10" s="12"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="E10" s="14"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
@@ -2152,82 +2559,94 @@
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="11"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="23"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="11"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="11"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>58</v>
+      </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="11"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="E18" s="14"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="11"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="A21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -2297,8 +2716,8 @@
   </sheetPr>
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2329,7 +2748,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -2338,14 +2757,18 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5">
-        <v>0.8962</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="22">
+        <v>0.69620000000000004</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.90380000000000005</v>
+      </c>
+      <c r="D3" s="25">
         <v>0.90580000000000005</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="30">
+        <v>0.86539999999999995</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
@@ -2353,14 +2776,18 @@
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9">
-        <v>0.83460000000000001</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="B4" s="22">
+        <v>0.90769999999999995</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.84230000000000005</v>
+      </c>
+      <c r="D4" s="22">
         <v>0.86150000000000004</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="23">
+        <v>0.8538</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
@@ -2368,14 +2795,18 @@
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
-        <v>0.9577</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="B5" s="22">
+        <v>0.48459999999999998</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.96540000000000004</v>
+      </c>
+      <c r="D5" s="22">
         <v>0.95</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="23">
+        <v>0.87690000000000001</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
@@ -2383,14 +2814,18 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
-        <v>0.88929999999999998</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="B6" s="22">
+        <v>0.74919999999999998</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="D6" s="22">
         <v>0.90139999999999998</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="23">
+        <v>0.86380000000000001</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
@@ -2398,14 +2833,18 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
-        <v>0.95179999999999998</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="B7" s="22">
+        <v>0.63780000000000003</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="D7" s="22">
         <v>0.94510000000000005</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="23">
+        <v>0.874</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
@@ -2413,14 +2852,18 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
-        <v>0.83460000000000001</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="B8" s="22">
+        <v>0.90769999999999995</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.84230000000000005</v>
+      </c>
+      <c r="D8" s="22">
         <v>0.86150000000000004</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="23">
+        <v>0.8538</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
@@ -2428,164 +2871,172 @@
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="10"/>
+      <c r="B9" s="27">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="27">
+        <v>0.95440000000000003</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.92889999999999995</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
-      <c r="B11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="26"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="29"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
@@ -2637,7 +3088,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E3" sqref="E3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2668,7 +3119,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -2677,12 +3128,18 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5">
+      <c r="B3" s="22">
+        <v>0.65090000000000003</v>
+      </c>
+      <c r="C3" s="25">
         <v>0.71479999999999999</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="25">
+        <v>0.68389999999999995</v>
+      </c>
+      <c r="E3" s="30">
+        <v>0.69320000000000004</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
@@ -2690,12 +3147,18 @@
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9">
+      <c r="B4" s="22">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="C4" s="22">
         <v>0.67390000000000005</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="22">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0.68820000000000003</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
@@ -2703,12 +3166,18 @@
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="B5" s="22">
+        <v>0.52869999999999995</v>
+      </c>
+      <c r="C5" s="22">
         <v>0.75570000000000004</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="22">
+        <v>0.70979999999999999</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.69830000000000003</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
@@ -2716,12 +3185,18 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
+      <c r="B6" s="22">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="C6" s="22">
         <v>0.7026</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="22">
+        <v>0.67549999999999999</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.69169999999999998</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
@@ -2729,12 +3204,18 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
+      <c r="B7" s="22">
+        <v>0.62119999999999997</v>
+      </c>
+      <c r="C7" s="22">
         <v>0.73399999999999999</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="22">
+        <v>0.69389999999999996</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.69520000000000004</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
@@ -2742,12 +3223,18 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
+      <c r="B8" s="22">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="C8" s="22">
         <v>0.67390000000000005</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="22">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.68820000000000003</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
@@ -2755,165 +3242,181 @@
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="10"/>
+      <c r="B9" s="27">
+        <v>0.72570000000000001</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="27">
+        <v>0.75109999999999999</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.76719999999999999</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="26"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="26"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="13"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="10"/>
+      <c r="A24" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
@@ -2955,8 +3458,8 @@
   </sheetPr>
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C20"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2987,7 +3490,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -2996,14 +3499,18 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5">
+      <c r="B3" s="22">
+        <v>0.62829999999999997</v>
+      </c>
+      <c r="C3" s="25">
         <v>0.68020000000000003</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="25">
         <v>0.67179999999999995</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="30">
+        <v>0.68089999999999995</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
@@ -3011,14 +3518,18 @@
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9">
+      <c r="B4" s="22">
+        <v>0.74329999999999996</v>
+      </c>
+      <c r="C4" s="22">
         <v>0.62409999999999999</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="22">
         <v>0.60170000000000001</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="23">
+        <v>0.65780000000000005</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
@@ -3026,14 +3537,18 @@
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="B5" s="22">
+        <v>0.51329999999999998</v>
+      </c>
+      <c r="C5" s="22">
         <v>0.73629999999999995</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="22">
         <v>0.7419</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="23">
+        <v>0.70409999999999995</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
@@ -3041,14 +3556,18 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
+      <c r="B6" s="22">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="C6" s="22">
         <v>0.66120000000000001</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="22">
         <v>0.64710000000000001</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="23">
+        <v>0.6734</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
@@ -3056,14 +3575,18 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
+      <c r="B7" s="22">
+        <v>0.60429999999999995</v>
+      </c>
+      <c r="C7" s="22">
         <v>0.70299999999999996</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="22">
         <v>0.69979999999999998</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="23">
+        <v>0.68969999999999998</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
@@ -3071,14 +3594,18 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
+      <c r="B8" s="22">
+        <v>0.74329999999999996</v>
+      </c>
+      <c r="C8" s="22">
         <v>0.62409999999999999</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="22">
         <v>0.60170000000000001</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="23">
+        <v>0.65780000000000005</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
@@ -3086,138 +3613,152 @@
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="10"/>
+      <c r="B9" s="27">
+        <v>0.70169999999999999</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="23">
+        <v>0.73629999999999995</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="26"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="26"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
+      <c r="A21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>
@@ -3287,7 +3828,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E3" sqref="E3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3318,7 +3859,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -3327,217 +3868,269 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5">
+      <c r="B3" s="22">
+        <v>0.63439999999999996</v>
+      </c>
+      <c r="C3" s="25">
         <v>0.71199999999999997</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="25">
+        <v>0.66769999999999996</v>
+      </c>
+      <c r="E3" s="30">
+        <v>0.69940000000000002</v>
+      </c>
+      <c r="F3" s="30"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9">
+      <c r="B4" s="22">
+        <v>0.75629999999999997</v>
+      </c>
+      <c r="C4" s="22">
         <v>0.64549999999999996</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
+      <c r="D4" s="22">
+        <v>0.65880000000000005</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0.67059999999999997</v>
+      </c>
+      <c r="F4" s="23"/>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="B5" s="22">
+        <v>0.51259999999999994</v>
+      </c>
+      <c r="C5" s="22">
         <v>0.77839999999999998</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="22">
+        <v>0.67649999999999999</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.72819999999999996</v>
+      </c>
+      <c r="F5" s="23"/>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
+      <c r="B6" s="22">
+        <v>0.67410000000000003</v>
+      </c>
+      <c r="C6" s="22">
         <v>0.6915</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="22">
+        <v>0.66469999999999996</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.6905</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
+      <c r="B7" s="22">
+        <v>0.60809999999999997</v>
+      </c>
+      <c r="C7" s="22">
         <v>0.74450000000000005</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="D7" s="22">
+        <v>0.67069999999999996</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.71160000000000001</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
+      <c r="B8" s="22">
+        <v>0.75629999999999997</v>
+      </c>
+      <c r="C8" s="22">
         <v>0.64549999999999996</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="22">
+        <v>0.65880000000000005</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.67059999999999997</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="27">
+        <v>0.72</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="27">
+        <v>0.74750000000000005</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.76119999999999999</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="11"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
+      <c r="A21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -3606,7 +4199,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E10" sqref="B3:E10"/>
+      <selection activeCell="E3" sqref="E3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3637,7 +4230,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -3646,187 +4239,271 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="31">
+        <v>0.69420000000000004</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0.75260000000000005</v>
+      </c>
+      <c r="D3" s="32">
+        <v>0.73880000000000001</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0.75070000000000003</v>
+      </c>
+      <c r="F3" s="30"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
+      <c r="B4" s="31">
+        <v>0.80049999999999999</v>
+      </c>
+      <c r="C4" s="31">
+        <v>0.7087</v>
+      </c>
+      <c r="D4" s="31">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="E4" s="31">
+        <v>0.7651</v>
+      </c>
+      <c r="F4" s="23"/>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="B5" s="31">
+        <v>0.58789999999999998</v>
+      </c>
+      <c r="C5" s="31">
+        <v>0.79659999999999997</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.77170000000000005</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.73619999999999997</v>
+      </c>
+      <c r="F5" s="23"/>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="B6" s="31">
+        <v>0.72360000000000002</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0.74119999999999997</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.73</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0.75419999999999998</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="B7" s="31">
+        <v>0.66020000000000001</v>
+      </c>
+      <c r="C7" s="31">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.75560000000000005</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.74360000000000004</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="B8" s="31">
+        <v>0.80049999999999999</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0.7087</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.7651</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="33">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.84189999999999998</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.80910000000000004</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0.83179999999999998</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="11"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="11"/>
+      <c r="A18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
+      <c r="A19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
+      <c r="A21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -3895,7 +4572,7 @@
   <dimension ref="A1:IV26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="B3:E11"/>
+      <selection activeCell="E3" sqref="E3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3926,7 +4603,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -3935,10 +4612,18 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="B3" s="22">
+        <v>0.62719999999999998</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.70579999999999998</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.66180000000000005</v>
+      </c>
+      <c r="E3" s="30">
+        <v>0.68979999999999997</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
@@ -3946,10 +4631,18 @@
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="22">
+        <v>0.69489999999999996</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.58430000000000004</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.53259999999999996</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0.60189999999999999</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
@@ -3957,10 +4650,18 @@
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="22">
+        <v>0.5595</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.82730000000000004</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.79110000000000003</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.77769999999999995</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
@@ -3968,10 +4669,18 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="22">
+        <v>0.65080000000000005</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.66510000000000002</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.61160000000000003</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.65990000000000004</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
@@ -3979,10 +4688,18 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="B7" s="22">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.77190000000000003</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.71830000000000005</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.73019999999999996</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
@@ -3990,10 +4707,18 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="22">
+        <v>0.69489999999999996</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.58430000000000004</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.53259999999999996</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.60189999999999999</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
@@ -4001,120 +4726,156 @@
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="10"/>
+      <c r="B9" s="27">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.77180000000000004</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.72740000000000005</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.75219999999999998</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="26"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="26"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14"/>
+      <c r="A18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
+      <c r="A19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
+      <c r="A21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>

</xml_diff>